<commit_message>
Updated data catalogue to reflect recent sources
</commit_message>
<xml_diff>
--- a/data/1_data-catalogue.xlsx
+++ b/data/1_data-catalogue.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniepeacock/Salmon Watersheds Dropbox/Stephanie Peacock/X Drive/1_PROJECTS/1_Active/State of Salmon/2 Data and Analysis/state-of-salmon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858C8C91-9704-6140-98D6-C6367EACB8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452DB968-40E6-3948-B205-107FE6DBC9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28140" yWindow="760" windowWidth="24000" windowHeight="17260" xr2:uid="{12FFA9A0-CC92-DA46-AD37-45E58BB63F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,15 +38,16 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={A48A0C62-4DA0-F342-A294-5966C68AB66E}</author>
+    <author>tc={00D9F620-65F8-1C4D-A5D2-C6A8B66011C7}</author>
   </authors>
   <commentList>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{A48A0C62-4DA0-F342-A294-5966C68AB66E}">
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00D9F620-65F8-1C4D-A5D2-C6A8B66011C7}">
       <text>
-        <t>[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Can not reasonably use TCCHUM until we get more than 10 years so sticking to expansion. Note that there are no NuSEDS Fraser chum records since 2020!</t>
+    After discussion with Antonio Velez-Espino, I removed reporting run size because CTC catch is not adjusted to the same indicator stocks and cannot be added to escapement.
+</t>
       </text>
     </comment>
   </commentList>
@@ -396,88 +397,6 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t>TCTR (22)-01 Appendix D20:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Taku River Escape. (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0432FF"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>2021</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - email sent to request update Apr8)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TCTR (22)-01 Appendix D20:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Taku River Total Run (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0432FF"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>2021</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - email sent to request update Apr8)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>YUKON JTC (23)-01 Table B11:</t>
     </r>
     <r>
@@ -819,36 +738,24 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Spawners plus catch from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TCCHINOOK Table A14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Total Fraser (sum of LC, Rel., IM)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCCHINOOK Table B6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Sum of escapement to indicator stocks </t>
     </r>
     <r>
       <rPr>
@@ -862,24 +769,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TCCHINOOK Table B6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Sum of escapement to indicator stocks </t>
+      <t xml:space="preserve">Sum of Interior Fraser coho CUs: Total Return* (provided by DFO on request) </t>
     </r>
     <r>
       <rPr>
@@ -892,8 +782,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Sum of Interior Fraser coho CUs: Total Return* (provided by DFO on request) </t>
+    <t>* Yes, total return is defined as "final spawner estimate plus fish removed from the system by SEP or FN"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sum of Interior Fraser coho CUs: Total Prefishery Abundance (provided by DFO on request) </t>
     </r>
     <r>
       <rPr>
@@ -906,11 +799,22 @@
     </r>
   </si>
   <si>
-    <t>* Yes, total return is defined as "final spawner estimate plus fish removed from the system by SEP or FN"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sum of Interior Fraser coho CUs: Total Prefishery Abundance (provided by DFO on request) </t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>TCCHINOOK Table B3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> NBC Escapements and terminal runs (Area 3: Nass R. Esc and t.run) </t>
     </r>
     <r>
       <rPr>
@@ -920,65 +824,6 @@
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>(2022)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>TCCHINOOK Table B3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> NBC Escapements and terminal runs (Area 3: Nass R. Esc and t.run) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0432FF"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>(2022)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TCCHINOOK Table B3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: NBC Escapements and terminal runs (Area 4: Skeena R. Total Esc) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0432FF"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>(2021)</t>
     </r>
   </si>
   <si>
@@ -1104,30 +949,160 @@
       <rPr>
         <b/>
         <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCCHUM Table 3-11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Fraser river escapement </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0432FF"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">(2022) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Spawners plus catch from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>TCCHUM Table 3-8 &amp; 3-9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>: Total commercial, FSC, recreational harvest of Fraser chum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
         <color theme="0" tint="-0.34998626667073579"/>
         <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TCCHUM Table 3-11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Fraser river escapement </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t xml:space="preserve">(2019) 
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0432FF"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCCHINOOK Table B3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: NBC Escapement  (Area 4: Skeena R. Total Esc) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0432FF"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(2021)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spawners plus catch from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCCHINOOK Table A14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Total Fraser (sum of LC, Rel., IM)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">(2022)
 </t>
     </r>
     <r>
@@ -1136,74 +1111,79 @@
         <color theme="1"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
-      <t>Expanded from spawner surveys</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0432FF"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>(2020)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Spawners plus catch from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TCCHUM Table 3-8 &amp; 3-9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Total commercial, FSC, recreational harvest of Fraser chum </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t xml:space="preserve">(2019)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>No data available</t>
+      <t xml:space="preserve">No data available </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCTR (22)-01 Appendix D20:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Taku River Escape. (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0432FF"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>2023)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCTR (22)-01 Appendix D20:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Taku River Total Run (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0432FF"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -1211,7 +1191,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1268,13 +1248,6 @@
       <name val="Aptos Narrow (Body)"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0" tint="-0.34998626667073579"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Aptos Narrow"/>
@@ -1282,15 +1255,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0" tint="-0.34998626667073579"/>
-      <name val="Aptos Narrow (Body)"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1508,12 +1495,54 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1535,49 +1564,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1925,8 +1912,9 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D18" dT="2024-04-09T17:08:45.23" personId="{102B22B8-225C-164F-84CB-2C9B771C2996}" id="{A48A0C62-4DA0-F342-A294-5966C68AB66E}">
-    <text>Can not reasonably use TCCHUM until we get more than 10 years so sticking to expansion. Note that there are no NuSEDS Fraser chum records since 2020!</text>
+  <threadedComment ref="C19" dT="2024-04-17T17:18:12.69" personId="{102B22B8-225C-164F-84CB-2C9B771C2996}" id="{00D9F620-65F8-1C4D-A5D2-C6A8B66011C7}">
+    <text xml:space="preserve">After discussion with Antonio Velez-Espino, I removed reporting run size because CTC catch is not adjusted to the same indicator stocks and cannot be added to escapement.
+</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1936,10 +1924,10 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1955,28 +1943,28 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="C1" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="43"/>
-      <c r="B3" s="42"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
@@ -1997,19 +1985,19 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="32" t="s">
@@ -2023,36 +2011,36 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="32"/>
       <c r="G5" s="32"/>
       <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="24" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>35</v>
@@ -2068,18 +2056,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A7" s="38"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>20</v>
@@ -2092,33 +2080,33 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="40" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
@@ -2137,43 +2125,43 @@
       <c r="G9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="30"/>
+      <c r="H9" s="44"/>
     </row>
     <row r="10" spans="1:10" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="24" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="28" t="s">
-        <v>61</v>
+      <c r="C10" s="42" t="s">
+        <v>58</v>
       </c>
       <c r="D10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="38" t="s">
         <v>43</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>45</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="29"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
@@ -2183,37 +2171,37 @@
       <c r="F11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="25"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="39"/>
     </row>
     <row r="12" spans="1:10" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>62</v>
+      <c r="C12" s="22" t="s">
+        <v>65</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>45</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
@@ -2229,36 +2217,36 @@
       <c r="F13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="35"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="40" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="13" t="s">
         <v>5</v>
       </c>
@@ -2277,39 +2265,39 @@
       <c r="G15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="40" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="11" t="s">
         <v>5</v>
       </c>
@@ -2328,70 +2316,70 @@
       <c r="G17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="27"/>
+      <c r="H17" s="41"/>
     </row>
-    <row r="18" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
+    <row r="18" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="45" t="s">
-        <v>67</v>
+        <v>54</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>48</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="120" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
+    <row r="19" spans="1:8" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>56</v>
+      <c r="C19" s="45" t="s">
+        <v>66</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="31"/>
+        <v>57</v>
+      </c>
+      <c r="F19" s="33"/>
       <c r="G19" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D20" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="34" t="s">
         <v>21</v>
       </c>
       <c r="F20" s="32" t="s">
@@ -2405,7 +2393,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="13" t="s">
         <v>5</v>
       </c>
@@ -2424,7 +2412,7 @@
     </row>
     <row r="23" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>25</v>
@@ -2446,11 +2434,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="B2:B3"/>
@@ -2467,17 +2466,6 @@
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
update data catalogue and rmd doc
</commit_message>
<xml_diff>
--- a/data/1_data-catalogue.xlsx
+++ b/data/1_data-catalogue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniepeacock/Salmon Watersheds Dropbox/Stephanie Peacock/X Drive/1_PROJECTS/1_Active/State of Salmon/2 Data and Analysis/state-of-salmon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452DB968-40E6-3948-B205-107FE6DBC9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0977ED-00DD-C145-BF05-56A8A0DE29A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28140" yWindow="760" windowWidth="24000" windowHeight="17260" xr2:uid="{12FFA9A0-CC92-DA46-AD37-45E58BB63F9E}"/>
+    <workbookView xWindow="-27360" yWindow="1280" windowWidth="24000" windowHeight="17260" xr2:uid="{12FFA9A0-CC92-DA46-AD37-45E58BB63F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,28 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={231B55C5-9633-E642-BA91-093A4D80FBD7}</author>
+    <author>tc={9137A95F-9B72-4E4B-9C67-9728464DE384}</author>
     <author>tc={00D9F620-65F8-1C4D-A5D2-C6A8B66011C7}</author>
   </authors>
   <commentList>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00D9F620-65F8-1C4D-A5D2-C6A8B66011C7}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{231B55C5-9633-E642-BA91-093A4D80FBD7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Expansion factors have been creeping up (3.5 in 2020, 4.5 in 2022) but still reasonable.</t>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="1" shapeId="0" xr:uid="{9137A95F-9B72-4E4B-9C67-9728464DE384}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Recent expansion factors are high (&gt;100 for 2015, 2016, 2019)</t>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="2" shapeId="0" xr:uid="{00D9F620-65F8-1C4D-A5D2-C6A8B66011C7}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>Chinook</t>
   </si>
@@ -1184,6 +1202,34 @@
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sum of total escapement (TE) across 3 CUs from English et al. (2023) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0432FF"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sum of total run size across 3 CUs from English et al (2023) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0432FF"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(2022)</t>
     </r>
   </si>
 </sst>
@@ -1495,9 +1541,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1555,16 +1598,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1912,6 +1958,12 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E12" dT="2024-04-18T15:43:15.71" personId="{102B22B8-225C-164F-84CB-2C9B771C2996}" id="{231B55C5-9633-E642-BA91-093A4D80FBD7}">
+    <text>Expansion factors have been creeping up (3.5 in 2020, 4.5 in 2022) but still reasonable.</text>
+  </threadedComment>
+  <threadedComment ref="C14" dT="2024-04-17T17:50:44.63" personId="{102B22B8-225C-164F-84CB-2C9B771C2996}" id="{9137A95F-9B72-4E4B-9C67-9728464DE384}">
+    <text>Recent expansion factors are high (&gt;100 for 2015, 2016, 2019)</text>
+  </threadedComment>
   <threadedComment ref="C19" dT="2024-04-17T17:18:12.69" personId="{102B22B8-225C-164F-84CB-2C9B771C2996}" id="{00D9F620-65F8-1C4D-A5D2-C6A8B66011C7}">
     <text xml:space="preserve">After discussion with Antonio Velez-Espino, I removed reporting run size because CTC catch is not adjusted to the same indicator stocks and cannot be added to escapement.
 </text>
@@ -1924,10 +1976,10 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1947,24 +1999,24 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
@@ -1985,7 +2037,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -1997,21 +2049,21 @@
       <c r="D4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="32" t="s">
+      <c r="E4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="31" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
@@ -2021,13 +2073,13 @@
       <c r="D5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -2056,7 +2108,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="13" t="s">
         <v>5</v>
       </c>
@@ -2080,7 +2132,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -2101,12 +2153,12 @@
       <c r="G8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="39" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
@@ -2125,63 +2177,63 @@
       <c r="G9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="44"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="43" t="s">
         <v>58</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>41</v>
+      <c r="E10" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="37" t="s">
         <v>43</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
+    <row r="11" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
       <c r="B11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="43"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>20</v>
+      <c r="E11" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="39"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="38"/>
     </row>
     <row r="12" spans="1:10" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="45" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -2193,7 +2245,7 @@
       <c r="F12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="36" t="s">
         <v>45</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -2201,7 +2253,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
@@ -2217,10 +2269,10 @@
       <c r="F13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="36"/>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2241,12 +2293,12 @@
       <c r="G14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="39" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="13" t="s">
         <v>5</v>
       </c>
@@ -2265,10 +2317,10 @@
       <c r="G15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="41"/>
+      <c r="H15" s="40"/>
     </row>
     <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -2289,7 +2341,7 @@
       <c r="G16" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -2297,7 +2349,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="11" t="s">
         <v>5</v>
       </c>
@@ -2316,10 +2368,10 @@
       <c r="G17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="41"/>
+      <c r="H17" s="40"/>
     </row>
     <row r="18" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -2328,13 +2380,13 @@
       <c r="C18" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="22" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="32" t="s">
         <v>48</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -2345,11 +2397,11 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="103" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="42" t="s">
         <v>66</v>
       </c>
       <c r="D19" s="15" t="s">
@@ -2358,7 +2410,7 @@
       <c r="E19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="33"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="1" t="s">
         <v>50</v>
       </c>
@@ -2367,7 +2419,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -2376,13 +2428,13 @@
       <c r="C20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="31" t="s">
         <v>21</v>
       </c>
       <c r="G20" s="7" t="s">
@@ -2393,16 +2445,16 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="25"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="3" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Update Skeena chinook esc to GSI
</commit_message>
<xml_diff>
--- a/data/1_data-catalogue.xlsx
+++ b/data/1_data-catalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniepeacock/Salmon Watersheds Dropbox/Stephanie Peacock/X Drive/1_PROJECTS/1_Active/State of Salmon/2 Data and Analysis/state-of-salmon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3828E41-6138-C943-910B-698E25271E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9958936D-095F-CD48-9019-493AEAFEF66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="1280" windowWidth="24000" windowHeight="17260" xr2:uid="{12FFA9A0-CC92-DA46-AD37-45E58BB63F9E}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="71">
   <si>
     <t>Chinook</t>
   </si>
@@ -1048,37 +1048,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TCCHINOOK Table B3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: NBC Escapement  (Area 4: Skeena R. Total Esc) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0432FF"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>(2021)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Spawners plus catch from </t>
     </r>
     <r>
@@ -1241,6 +1210,37 @@
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>(2023)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCCHINOOK Table B3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: NBC Escapement  (Area 4: Skeena R. GSI esc) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0432FF"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(2022)</t>
     </r>
   </si>
 </sst>
@@ -1981,10 +1981,10 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2097,7 +2097,7 @@
         <v>35</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>34</v>
@@ -2124,7 +2124,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>20</v>
@@ -2198,7 +2198,7 @@
         <v>40</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>40</v>
@@ -2223,7 +2223,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>20</v>
@@ -2239,7 +2239,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>45</v>
@@ -2346,8 +2346,8 @@
       <c r="G16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="27" t="s">
-        <v>20</v>
+      <c r="H16" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>52</v>
@@ -2373,7 +2373,9 @@
       <c r="G17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="28"/>
+      <c r="H17" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
@@ -2407,7 +2409,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>63</v>
@@ -2446,7 +2448,7 @@
         <v>22</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -2495,7 +2497,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="26">
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="B2:B3"/>
@@ -2512,7 +2514,6 @@
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="F18:F19"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="F20:F21"/>
@@ -2520,9 +2521,9 @@
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="H8:H9"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>